<commit_message>
Incorporate the results of David Holman's latest PEST calibration of Mehama37. HBV.csv - Incorporate new calibration of Mehama37. FLOWreports_NSantiam.xml - Add a monthly version of the FLOW NSantiam Reach Exchanges report. Add a FLOWreports_WRB.xml file.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_WRB.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_WRB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CW3M\trunk\DataCW3M\RegressionTesting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55679ED-A866-475A-BD45-A5B31E13DD3C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63209CC8-7A99-4CE5-877F-4352BD1C98BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2370" yWindow="2595" windowWidth="21600" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -45,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="54">
   <si>
     <t>Year</t>
   </si>
@@ -198,6 +201,15 @@
   </si>
   <si>
     <t>CW3M c194</t>
+  </si>
+  <si>
+    <t>Demo_Baseline 5/20/21</t>
+  </si>
+  <si>
+    <t>CW3M ~C401</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> water added by FlowModel (mm)</t>
   </si>
 </sst>
 </file>
@@ -1161,21 +1173,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B50F6A88-D908-47A2-AF67-31CE5DBD8EA6}">
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="43.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="4" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" customWidth="1"/>
+    <col min="4" max="13" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="135" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1226,7 +1238,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>15</v>
       </c>
@@ -1273,7 +1285,7 @@
         <v>-9.5399999999999999E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -1320,7 +1332,7 @@
         <v>-9.5399999999999999E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1370,7 +1382,7 @@
         <v>-6.5600000000000001E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>37</v>
       </c>
@@ -1423,7 +1435,7 @@
         <v>-5.5199999999999997E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>39</v>
       </c>
@@ -1476,7 +1488,7 @@
         <v>-5.5199999999999997E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>42</v>
       </c>
@@ -1529,7 +1541,7 @@
         <v>-5.5199999999999997E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>50</v>
       </c>
@@ -1582,7 +1594,7 @@
         <v>-6.0499999999999996E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -1597,7 +1609,7 @@
       <c r="O9" s="4"/>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1647,7 +1659,7 @@
         <v>-6.6799999999999997E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1697,7 +1709,7 @@
         <v>-7.7676100000000005E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>32</v>
       </c>
@@ -1744,13 +1756,13 @@
         <v>3.1494380141050674E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="J13" s="12">
         <f>(K12+J12)/E12</f>
         <v>0.43720161777754918</v>
       </c>
     </row>
-    <row r="14" spans="1:19" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" s="1" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>32</v>
       </c>
@@ -1798,7 +1810,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>2010</v>
       </c>
@@ -1864,14 +1876,14 @@
       <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="42.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -1924,7 +1936,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1977,7 +1989,7 @@
         <v>-3.3387499999999997E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -2030,7 +2042,7 @@
         <v>-3.6450000000000002E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2083,7 +2095,7 @@
         <v>-3.5375000000000001E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -2136,7 +2148,7 @@
         <v>-3.3537500000000006E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D6" s="3"/>
       <c r="E6" s="14"/>
       <c r="F6" s="3"/>
@@ -2152,7 +2164,7 @@
       <c r="P6" s="3"/>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D7" s="3"/>
       <c r="E7" s="14"/>
       <c r="F7" s="3"/>
@@ -2168,7 +2180,7 @@
       <c r="P7" s="3"/>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -2222,7 +2234,7 @@
       </c>
       <c r="V8" s="16"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -2277,7 +2289,7 @@
         <v>1.0904389977311683E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -2293,7 +2305,7 @@
       <c r="P10" s="3"/>
       <c r="Q10" s="5"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -2346,7 +2358,7 @@
         <v>-2.2650000000000003E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -2399,7 +2411,7 @@
         <v>-3.02347125E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="150" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
       <c r="C14" s="9" t="s">
         <v>0</v>
       </c>
@@ -2446,7 +2458,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>29</v>
       </c>
@@ -2496,7 +2508,7 @@
         <v>285638.625</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C16" s="8" t="s">
         <v>43</v>
       </c>
@@ -2544,7 +2556,7 @@
       </c>
       <c r="R16" s="4"/>
     </row>
-    <row r="21" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D21" s="3">
         <v>1059.3576249999999</v>
       </c>
@@ -2595,20 +2607,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F1D315-50C2-4E05-943E-CA7A96C8E688}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:Q2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="42.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="8" customWidth="1"/>
+    <col min="18" max="18" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -2634,34 +2647,37 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -2686,35 +2702,36 @@
       <c r="H2" s="3">
         <v>5.2671874444444455</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="3"/>
+      <c r="J2" s="3">
         <v>2.7783584444444447</v>
       </c>
-      <c r="J2" s="3">
+      <c r="K2" s="3">
         <v>645.94646555555562</v>
       </c>
-      <c r="K2" s="3">
+      <c r="L2" s="3">
         <v>46.522305444444449</v>
       </c>
-      <c r="L2" s="3">
+      <c r="M2" s="3">
         <v>1071.222696888889</v>
       </c>
-      <c r="M2" s="3">
+      <c r="N2" s="3">
         <v>1367.005249</v>
       </c>
-      <c r="N2" s="4">
+      <c r="O2" s="4">
         <v>324487.69965277775</v>
       </c>
-      <c r="O2" s="4">
+      <c r="P2" s="4">
         <v>286418.88888888888</v>
       </c>
-      <c r="P2" s="3">
+      <c r="Q2" s="3">
         <v>-1.3017665555555555</v>
       </c>
-      <c r="Q2" s="5">
+      <c r="R2" s="5">
         <v>-4.1888888888888895E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -2739,32 +2756,89 @@
       <c r="H3" s="3">
         <v>5.2671874444444455</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="3"/>
+      <c r="J3" s="3">
         <v>2.7783584444444447</v>
       </c>
-      <c r="J3" s="3">
+      <c r="K3" s="3">
         <v>649.53888622222212</v>
       </c>
-      <c r="K3" s="3">
+      <c r="L3" s="3">
         <v>46.522305444444449</v>
       </c>
-      <c r="L3" s="3">
+      <c r="M3" s="3">
         <v>1061.188924111111</v>
       </c>
-      <c r="M3" s="3">
+      <c r="N3" s="3">
         <v>1394.2609456666667</v>
       </c>
-      <c r="N3" s="4">
+      <c r="O3" s="4">
         <v>321964.87847222225</v>
       </c>
-      <c r="O3" s="4">
+      <c r="P3" s="4">
         <v>286416.86805555556</v>
       </c>
-      <c r="P3" s="3">
+      <c r="Q3" s="3">
         <v>-1.2769506666666668</v>
       </c>
-      <c r="Q3" s="5">
+      <c r="R3" s="5">
         <v>-4.0766666666666664E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1150.0584241111112</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1612.6987305555554</v>
+      </c>
+      <c r="F4" s="6">
+        <v>14.557748111111115</v>
+      </c>
+      <c r="G4" s="6">
+        <v>52.671807666666659</v>
+      </c>
+      <c r="H4" s="3">
+        <v>5.2565644444444439</v>
+      </c>
+      <c r="I4" s="6">
+        <v>8.9746754444444452</v>
+      </c>
+      <c r="J4" s="14">
+        <v>2.782013222222222</v>
+      </c>
+      <c r="K4" s="6">
+        <v>609.74378122222208</v>
+      </c>
+      <c r="L4" s="3">
+        <v>44.391417555555549</v>
+      </c>
+      <c r="M4" s="6">
+        <v>1018.5836656666668</v>
+      </c>
+      <c r="N4" s="6">
+        <v>1167.9530299999999</v>
+      </c>
+      <c r="O4" s="7">
+        <v>517762.13888888888</v>
+      </c>
+      <c r="P4" s="4">
+        <v>286785.73958333331</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>-0.76404255555555545</v>
+      </c>
+      <c r="R4" s="5">
+        <v>-2.7444444444444445E-4</v>
       </c>
     </row>
   </sheetData>
@@ -2780,16 +2854,16 @@
       <selection activeCell="P4" sqref="P4:Q4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="15" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="15" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -2842,7 +2916,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -2895,7 +2969,7 @@
         <v>-1.2809E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -2950,7 +3024,7 @@
         <v>8.9706148445115703E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -3005,7 +3079,7 @@
         <v>9.4838660254976705E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="115.2" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
         <v>47</v>
       </c>
@@ -3052,7 +3126,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D7" s="3">
         <v>1058.7642000000001</v>
       </c>
@@ -3109,12 +3183,12 @@
       <selection sqref="A1:O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>2010</v>
       </c>
@@ -3161,7 +3235,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -3208,7 +3282,7 @@
         <v>-9.5399999999999999E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -3255,7 +3329,7 @@
         <v>-7.2000000000000005E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -3315,26 +3389,26 @@
       <selection activeCell="O10" sqref="A10:O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="43.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="43.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="35.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3381,7 +3455,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2010</v>
       </c>
@@ -3428,7 +3502,7 @@
         <v>-7.2000000000000005E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2011</v>
       </c>
@@ -3475,7 +3549,7 @@
         <v>-2.2880000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2012</v>
       </c>
@@ -3522,7 +3596,7 @@
         <v>1.8749999999999999E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2013</v>
       </c>
@@ -3569,7 +3643,7 @@
         <v>-2.0699999999999999E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2014</v>
       </c>
@@ -3616,7 +3690,7 @@
         <v>-1.76E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2015</v>
       </c>
@@ -3663,7 +3737,7 @@
         <v>-2.1599999999999999E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2016</v>
       </c>
@@ -3710,7 +3784,7 @@
         <v>-8.6000000000000003E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2017</v>
       </c>
@@ -3757,7 +3831,7 @@
         <v>-1.2E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -3834,9 +3908,9 @@
       <selection activeCell="B2" sqref="B2:O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3883,7 +3957,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2010</v>
       </c>
@@ -3930,7 +4004,7 @@
         <v>-9.5399999999999999E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2011</v>
       </c>
@@ -3977,7 +4051,7 @@
         <v>-1.307E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2012</v>
       </c>
@@ -4024,7 +4098,7 @@
         <v>1.2149999999999999E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2013</v>
       </c>
@@ -4071,7 +4145,7 @@
         <v>-1.07E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2014</v>
       </c>
@@ -4118,7 +4192,7 @@
         <v>-5.1E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2015</v>
       </c>
@@ -4165,7 +4239,7 @@
         <v>-8.6200000000000003E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2016</v>
       </c>
@@ -4212,7 +4286,7 @@
         <v>-1.46E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2017</v>
       </c>
@@ -4259,7 +4333,7 @@
         <v>-4.5899999999999999E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Commit additions to documentation regarding water rights. wr_pods.csv - Correct an error found by Doug Quirke. FLOWreports_WRB.xml - Add "FLOW WRB-NSantiam temperature skill assessment monthly" report.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_WRB.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_WRB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27446361-0709-4C0B-93F2-79E264338ABE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0613D69-FBD6-4317-A293-7208460EA862}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2616,7 +2616,7 @@
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2861,13 +2861,13 @@
         <v>1150.4691636666666</v>
       </c>
       <c r="E5" s="3">
-        <v>1612.6987305555554</v>
+        <v>1612.6987305555599</v>
       </c>
       <c r="F5" s="3">
-        <v>14.557834333333334</v>
+        <v>14.5578343333333</v>
       </c>
       <c r="G5" s="3">
-        <v>52.671807666666659</v>
+        <v>52.671807666666702</v>
       </c>
       <c r="H5" s="3">
         <v>5.2565644444444439</v>

</xml_diff>

<commit_message>
CW3M_WRB.envx - Turn off coldstart. Observations - Add the observations for gages on the Willamette mainstem. Reporter_SSantiam.xml - Fix a syntax error. FLOWreports_WRB.xml - Remove unneeded stuff.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_WRB.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_WRB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3DF0F3-6206-41CD-A4B6-8B6EFCE9A210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03F3C0B-C436-4EBE-9E26-DB76DA61AFFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010" sheetId="5" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="59">
   <si>
     <t>Year</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>CW3M C492</t>
+  </si>
+  <si>
+    <t>CW3M C577</t>
   </si>
 </sst>
 </file>
@@ -1189,17 +1192,17 @@
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="43.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="4" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" customWidth="1"/>
+    <col min="4" max="13" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="135" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1250,7 +1253,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>15</v>
       </c>
@@ -1297,7 +1300,7 @@
         <v>-9.5399999999999999E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -1344,7 +1347,7 @@
         <v>-9.5399999999999999E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1394,7 +1397,7 @@
         <v>-6.5600000000000001E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>37</v>
       </c>
@@ -1447,7 +1450,7 @@
         <v>-5.5199999999999997E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>39</v>
       </c>
@@ -1500,7 +1503,7 @@
         <v>-5.5199999999999997E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>42</v>
       </c>
@@ -1553,7 +1556,7 @@
         <v>-5.5199999999999997E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>50</v>
       </c>
@@ -1606,7 +1609,7 @@
         <v>-6.0499999999999996E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -1621,7 +1624,7 @@
       <c r="O9" s="4"/>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1671,7 +1674,7 @@
         <v>-6.6799999999999997E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1721,7 +1724,7 @@
         <v>-7.7676100000000005E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>32</v>
       </c>
@@ -1768,13 +1771,13 @@
         <v>3.1494380141050674E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="J13" s="12">
         <f>(K12+J12)/E12</f>
         <v>0.43720161777754918</v>
       </c>
     </row>
-    <row r="14" spans="1:19" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" s="1" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>32</v>
       </c>
@@ -1822,7 +1825,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>2010</v>
       </c>
@@ -1888,14 +1891,14 @@
       <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="42.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -1948,7 +1951,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2001,7 +2004,7 @@
         <v>-3.3387499999999997E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -2054,7 +2057,7 @@
         <v>-3.6450000000000002E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2107,7 +2110,7 @@
         <v>-3.5375000000000001E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -2160,7 +2163,7 @@
         <v>-3.3537500000000006E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D6" s="3"/>
       <c r="E6" s="14"/>
       <c r="F6" s="3"/>
@@ -2176,7 +2179,7 @@
       <c r="P6" s="3"/>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D7" s="3"/>
       <c r="E7" s="14"/>
       <c r="F7" s="3"/>
@@ -2192,7 +2195,7 @@
       <c r="P7" s="3"/>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -2246,7 +2249,7 @@
       </c>
       <c r="V8" s="16"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -2301,7 +2304,7 @@
         <v>1.0904389977311683E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -2317,7 +2320,7 @@
       <c r="P10" s="3"/>
       <c r="Q10" s="5"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -2370,7 +2373,7 @@
         <v>-2.2650000000000003E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -2423,7 +2426,7 @@
         <v>-3.02347125E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="150" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
       <c r="C14" s="9" t="s">
         <v>0</v>
       </c>
@@ -2470,7 +2473,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>29</v>
       </c>
@@ -2520,7 +2523,7 @@
         <v>285638.625</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C16" s="8" t="s">
         <v>43</v>
       </c>
@@ -2568,7 +2571,7 @@
       </c>
       <c r="R16" s="4"/>
     </row>
-    <row r="21" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D21" s="3">
         <v>1059.3576249999999</v>
       </c>
@@ -2619,27 +2622,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F1D315-50C2-4E05-943E-CA7A96C8E688}">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="42.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="8" customWidth="1"/>
-    <col min="18" max="18" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="8" customWidth="1"/>
+    <col min="18" max="18" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="C1" s="9" t="s">
         <v>22</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>-4.1888888888888895E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>-4.0766666666666664E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>-2.7444444444444445E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>-2.7411111111111109E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -2965,7 +2965,7 @@
         <v>-2.7177777777777774E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -3019,6 +3019,62 @@
       </c>
       <c r="R7" s="5">
         <v>-2.8644444444444442E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1181.5808646666667</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1612.6987305555554</v>
+      </c>
+      <c r="F8" s="3">
+        <v>14.207868333333332</v>
+      </c>
+      <c r="G8" s="3">
+        <v>52.671807666666659</v>
+      </c>
+      <c r="H8" s="3">
+        <v>5.2579661111111111</v>
+      </c>
+      <c r="I8" s="3">
+        <v>8.7714771111111105</v>
+      </c>
+      <c r="J8" s="3">
+        <v>2.7833133333333331</v>
+      </c>
+      <c r="K8" s="6">
+        <v>592.07319488888891</v>
+      </c>
+      <c r="L8" s="6">
+        <v>43.587652666666663</v>
+      </c>
+      <c r="M8" s="6">
+        <v>1035.3851454444443</v>
+      </c>
+      <c r="N8" s="6">
+        <v>1200.5520154444446</v>
+      </c>
+      <c r="O8" s="7">
+        <v>505160.02083333331</v>
+      </c>
+      <c r="P8" s="4">
+        <v>286902.89236111112</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>-0.80739277777777785</v>
+      </c>
+      <c r="R8" s="5">
+        <v>-2.8255555555555559E-4</v>
       </c>
     </row>
   </sheetData>
@@ -3034,16 +3090,16 @@
       <selection activeCell="P4" sqref="P4:Q4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="15" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="15" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -3096,7 +3152,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -3149,7 +3205,7 @@
         <v>-1.2809E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -3204,7 +3260,7 @@
         <v>8.9706148445115703E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -3259,7 +3315,7 @@
         <v>9.4838660254976705E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="115.2" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
         <v>47</v>
       </c>
@@ -3306,7 +3362,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D7" s="3">
         <v>1058.7642000000001</v>
       </c>
@@ -3363,12 +3419,12 @@
       <selection sqref="A1:O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>2010</v>
       </c>
@@ -3415,7 +3471,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -3462,7 +3518,7 @@
         <v>-9.5399999999999999E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -3509,7 +3565,7 @@
         <v>-7.2000000000000005E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -3569,26 +3625,26 @@
       <selection activeCell="O10" sqref="A10:O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="43.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="43.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="35.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3635,7 +3691,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2010</v>
       </c>
@@ -3682,7 +3738,7 @@
         <v>-7.2000000000000005E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2011</v>
       </c>
@@ -3729,7 +3785,7 @@
         <v>-2.2880000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2012</v>
       </c>
@@ -3776,7 +3832,7 @@
         <v>1.8749999999999999E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2013</v>
       </c>
@@ -3823,7 +3879,7 @@
         <v>-2.0699999999999999E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2014</v>
       </c>
@@ -3870,7 +3926,7 @@
         <v>-1.76E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2015</v>
       </c>
@@ -3917,7 +3973,7 @@
         <v>-2.1599999999999999E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2016</v>
       </c>
@@ -3964,7 +4020,7 @@
         <v>-8.6000000000000003E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2017</v>
       </c>
@@ -4011,7 +4067,7 @@
         <v>-1.2E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -4088,9 +4144,9 @@
       <selection activeCell="B2" sqref="B2:O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4137,7 +4193,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2010</v>
       </c>
@@ -4184,7 +4240,7 @@
         <v>-9.5399999999999999E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2011</v>
       </c>
@@ -4231,7 +4287,7 @@
         <v>-1.307E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2012</v>
       </c>
@@ -4278,7 +4334,7 @@
         <v>1.2149999999999999E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2013</v>
       </c>
@@ -4325,7 +4381,7 @@
         <v>-1.07E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2014</v>
       </c>
@@ -4372,7 +4428,7 @@
         <v>-5.1E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2015</v>
       </c>
@@ -4419,7 +4475,7 @@
         <v>-8.6200000000000003E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2016</v>
       </c>
@@ -4466,7 +4522,7 @@
         <v>-1.46E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2017</v>
       </c>
@@ -4513,7 +4569,7 @@
         <v>-4.5899999999999999E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
CW3M_Quartzville53_2010-2018.pst - Change paths from \CW3M_McKenzie_1.1.0\ to C:\CW3M.git\trunk\DataCW3M\. SimulationScenarios_PEST.xml - Comment out the PEST_Spinup scenario. Add SkillWRB.xlsx in the SkillAssessment folder. Reporter_SSantiam.xml - Fix a syntax error.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_WRB.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_WRB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03F3C0B-C436-4EBE-9E26-DB76DA61AFFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FEA653-1457-4D11-9C6D-5CD808A8CFF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="60">
   <si>
     <t>Year</t>
   </si>
@@ -224,7 +224,10 @@
     <t>CW3M C492</t>
   </si>
   <si>
-    <t>CW3M C577</t>
+    <t>CW3M C579</t>
+  </si>
+  <si>
+    <t>CW3M C584</t>
   </si>
 </sst>
 </file>
@@ -2622,10 +2625,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F1D315-50C2-4E05-943E-CA7A96C8E688}">
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3074,6 +3077,62 @@
         <v>-0.80739277777777785</v>
       </c>
       <c r="R8" s="5">
+        <v>-2.8255555555555559E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1181.5808646666667</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1612.6987305555554</v>
+      </c>
+      <c r="F9" s="3">
+        <v>14.207868333333332</v>
+      </c>
+      <c r="G9" s="3">
+        <v>52.671807666666659</v>
+      </c>
+      <c r="H9" s="3">
+        <v>5.2579661111111111</v>
+      </c>
+      <c r="I9" s="3">
+        <v>8.7714771111111105</v>
+      </c>
+      <c r="J9" s="3">
+        <v>2.7833133333333331</v>
+      </c>
+      <c r="K9" s="3">
+        <v>592.07319488888891</v>
+      </c>
+      <c r="L9" s="3">
+        <v>43.587652666666663</v>
+      </c>
+      <c r="M9" s="3">
+        <v>1035.3851454444443</v>
+      </c>
+      <c r="N9" s="3">
+        <v>1200.5520154444446</v>
+      </c>
+      <c r="O9" s="4">
+        <v>505160.02083333331</v>
+      </c>
+      <c r="P9" s="4">
+        <v>286902.89236111112</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>-0.80739277777777785</v>
+      </c>
+      <c r="R9" s="5">
         <v>-2.8255555555555559E-4</v>
       </c>
     </row>

</xml_diff>